<commit_message>
Excel read and write
</commit_message>
<xml_diff>
--- a/src/test/ExcelFiles/Book1.xlsx
+++ b/src/test/ExcelFiles/Book1.xlsx
@@ -1,26 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\armac\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\armac\IdeaProjects\Mysql_Excel_Project4\src\test\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF2294A-8F7E-4B7C-87EC-4DD6A9A54282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EE3B01-A331-47B2-A9BE-D1258D455F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
+    <sheet name="Employees" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Armachen Anbessa</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>arma@gmail.com</t>
+  </si>
+  <si>
+    <t>456 Addis</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -366,14 +390,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>